<commit_message>
1. input passive table
</commit_message>
<xml_diff>
--- a/Assets/Resources/Excel/PassiveSkillDataExcel.xlsx
+++ b/Assets/Resources/Excel/PassiveSkillDataExcel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Id</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -66,15 +66,1149 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>test</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>test</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>test</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>강화</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>철판</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>강화</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>탄두</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>치명</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>탄두</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>어뢰</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>갑판</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>대공</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>부포</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>빠른</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>장정</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>명중</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>강화</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>전선</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>구축</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>함체 구축</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>파괴자</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>강철</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>철판</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>강철</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>탄두</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>치명</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>철탄</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>어뢰</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>강철판</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>강철</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>대공</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>부포</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>더</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>빠른</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>장전</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>향상된</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>집중력</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>함체</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>보강</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>금갑판</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>광기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>장인의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>철갑</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>장인의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>탄두</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>장인의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>센서</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>장인의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>부포</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>장인의 조타</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>장인의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>장탄</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>치명적인</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>타격</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>강심장</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>적대심</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>지원요청</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>명장의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>철판</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>명장의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>탄두</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>명장의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>운</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>명장의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>장탄</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>살신</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>성인</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>동귀어진</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>지피지기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>금강불체</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>하늘의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지배자</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>바다의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지배자</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>증명</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>불법개조</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>영웅심리</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>어뢰왕</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>해적</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>귀족</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>저격왕</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>매의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>눈</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>황금함대</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>피빛함대</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>대장선</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>부활</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>집중</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF373A3C"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>사격</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>유령선</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>반격</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>지원선</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>해골선</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>위장</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>패황</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>초신성</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -82,7 +1216,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,8 +1250,15 @@
       <name val="Open Sans"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF373A3C"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,8 +1283,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -166,13 +1343,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -195,6 +1409,69 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -477,10 +1754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T42"/>
+  <dimension ref="A1:T61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K55" sqref="K55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -542,28 +1819,28 @@
     </row>
     <row r="2" spans="1:20" ht="17.25" thickBot="1">
       <c r="A2" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="7">
-        <v>0</v>
-      </c>
-      <c r="E2" s="7">
-        <v>0</v>
-      </c>
-      <c r="F2" s="7">
-        <v>0</v>
-      </c>
-      <c r="G2" s="7">
+      <c r="C2" s="8" t="s">
         <v>10</v>
       </c>
+      <c r="D2" s="15">
+        <v>0</v>
+      </c>
+      <c r="E2" s="15">
+        <v>0</v>
+      </c>
+      <c r="F2" s="15">
+        <v>0</v>
+      </c>
+      <c r="G2" s="15">
+        <v>15</v>
+      </c>
       <c r="H2" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I2" s="7">
         <v>0</v>
@@ -584,28 +1861,28 @@
     </row>
     <row r="3" spans="1:20" ht="17.25" thickBot="1">
       <c r="A3" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="7">
-        <v>0</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0</v>
-      </c>
-      <c r="F3" s="7">
-        <v>0</v>
-      </c>
-      <c r="G3" s="7">
+      <c r="D3" s="15">
+        <v>0</v>
+      </c>
+      <c r="E3" s="15">
+        <v>0</v>
+      </c>
+      <c r="F3" s="15">
+        <v>1</v>
+      </c>
+      <c r="G3" s="15">
         <v>10</v>
       </c>
       <c r="H3" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I3" s="7">
         <v>0</v>
@@ -626,28 +1903,28 @@
     </row>
     <row r="4" spans="1:20" ht="17.25" thickBot="1">
       <c r="A4" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="7">
-        <v>0</v>
-      </c>
-      <c r="E4" s="7">
-        <v>0</v>
-      </c>
-      <c r="F4" s="7">
-        <v>0</v>
-      </c>
-      <c r="G4" s="7">
-        <v>10</v>
+      <c r="C4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="15">
+        <v>0</v>
+      </c>
+      <c r="E4" s="15">
+        <v>0</v>
+      </c>
+      <c r="F4" s="15">
+        <v>2</v>
+      </c>
+      <c r="G4" s="15">
+        <v>15</v>
       </c>
       <c r="H4" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I4" s="7">
         <v>0</v>
@@ -668,28 +1945,28 @@
     </row>
     <row r="5" spans="1:20" ht="17.25" thickBot="1">
       <c r="A5" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="7">
-        <v>0</v>
-      </c>
-      <c r="E5" s="7">
-        <v>0</v>
-      </c>
-      <c r="F5" s="7">
-        <v>0</v>
-      </c>
-      <c r="G5" s="7">
-        <v>10</v>
+      <c r="C5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="15">
+        <v>0</v>
+      </c>
+      <c r="E5" s="15">
+        <v>0</v>
+      </c>
+      <c r="F5" s="15">
+        <v>3</v>
+      </c>
+      <c r="G5" s="15">
+        <v>20</v>
       </c>
       <c r="H5" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I5" s="7">
         <v>0</v>
@@ -710,28 +1987,28 @@
     </row>
     <row r="6" spans="1:20" ht="17.25" thickBot="1">
       <c r="A6" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4">
         <v>1</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="7">
-        <v>0</v>
-      </c>
-      <c r="E6" s="7">
-        <v>0</v>
-      </c>
-      <c r="F6" s="7">
-        <v>0</v>
-      </c>
-      <c r="G6" s="7">
-        <v>10</v>
+      <c r="C6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="15">
+        <v>0</v>
+      </c>
+      <c r="E6" s="15">
+        <v>0</v>
+      </c>
+      <c r="F6" s="15">
+        <v>4</v>
+      </c>
+      <c r="G6" s="15">
+        <v>20</v>
       </c>
       <c r="H6" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I6" s="7">
         <v>0</v>
@@ -752,28 +2029,28 @@
     </row>
     <row r="7" spans="1:20" ht="17.25" thickBot="1">
       <c r="A7" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="7">
-        <v>0</v>
-      </c>
-      <c r="E7" s="7">
-        <v>0</v>
-      </c>
-      <c r="F7" s="7">
-        <v>0</v>
-      </c>
-      <c r="G7" s="7">
-        <v>10</v>
+      <c r="C7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="15">
+        <v>0</v>
+      </c>
+      <c r="E7" s="15">
+        <v>0</v>
+      </c>
+      <c r="F7" s="15">
+        <v>5</v>
+      </c>
+      <c r="G7" s="15">
+        <v>30</v>
       </c>
       <c r="H7" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I7" s="7">
         <v>0</v>
@@ -794,28 +2071,28 @@
     </row>
     <row r="8" spans="1:20" ht="17.25" thickBot="1">
       <c r="A8" s="6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="7">
-        <v>0</v>
-      </c>
-      <c r="E8" s="7">
-        <v>0</v>
-      </c>
-      <c r="F8" s="7">
-        <v>0</v>
-      </c>
-      <c r="G8" s="7">
-        <v>10</v>
+      <c r="C8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="15">
+        <v>0</v>
+      </c>
+      <c r="E8" s="15">
+        <v>0</v>
+      </c>
+      <c r="F8" s="15">
+        <v>6</v>
+      </c>
+      <c r="G8" s="15">
+        <v>25</v>
       </c>
       <c r="H8" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I8" s="7">
         <v>0</v>
@@ -836,28 +2113,28 @@
     </row>
     <row r="9" spans="1:20" ht="17.25" thickBot="1">
       <c r="A9" s="6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4">
         <v>1</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="7">
-        <v>0</v>
-      </c>
-      <c r="E9" s="7">
-        <v>0</v>
-      </c>
-      <c r="F9" s="7">
-        <v>0</v>
-      </c>
-      <c r="G9" s="7">
-        <v>10</v>
+      <c r="C9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="15">
+        <v>0</v>
+      </c>
+      <c r="E9" s="15">
+        <v>0</v>
+      </c>
+      <c r="F9" s="15">
+        <v>7</v>
+      </c>
+      <c r="G9" s="15">
+        <v>30</v>
       </c>
       <c r="H9" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I9" s="7">
         <v>0</v>
@@ -878,28 +2155,28 @@
     </row>
     <row r="10" spans="1:20" ht="17.25" thickBot="1">
       <c r="A10" s="6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4">
         <v>1</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="15">
+        <v>0</v>
+      </c>
+      <c r="E10" s="15">
+        <v>0</v>
+      </c>
+      <c r="F10" s="15">
+        <v>8</v>
+      </c>
+      <c r="G10" s="15">
         <v>10</v>
       </c>
-      <c r="D10" s="7">
-        <v>0</v>
-      </c>
-      <c r="E10" s="7">
-        <v>0</v>
-      </c>
-      <c r="F10" s="7">
-        <v>0</v>
-      </c>
-      <c r="G10" s="7">
-        <v>10</v>
-      </c>
       <c r="H10" s="7">
-        <v>5.5</v>
+        <v>100</v>
       </c>
       <c r="I10" s="7">
         <v>0</v>
@@ -920,28 +2197,28 @@
     </row>
     <row r="11" spans="1:20" ht="17.25" thickBot="1">
       <c r="A11" s="6">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="4">
         <v>1</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="7">
-        <v>0</v>
-      </c>
-      <c r="E11" s="7">
-        <v>0</v>
-      </c>
-      <c r="F11" s="7">
-        <v>0</v>
-      </c>
-      <c r="G11" s="7">
-        <v>10</v>
+      <c r="C11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="15">
+        <v>0</v>
+      </c>
+      <c r="E11" s="15">
+        <v>0</v>
+      </c>
+      <c r="F11" s="15">
+        <v>9</v>
+      </c>
+      <c r="G11" s="15">
+        <v>100</v>
       </c>
       <c r="H11" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I11" s="7">
         <v>0</v>
@@ -962,28 +2239,28 @@
     </row>
     <row r="12" spans="1:20" ht="17.25" thickBot="1">
       <c r="A12" s="6">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="4">
         <v>2</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="7">
-        <v>0</v>
-      </c>
-      <c r="E12" s="7">
-        <v>0</v>
-      </c>
-      <c r="F12" s="7">
-        <v>0</v>
-      </c>
-      <c r="G12" s="7">
-        <v>10</v>
+      <c r="C12" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="20">
+        <v>0</v>
+      </c>
+      <c r="E12" s="20">
+        <v>0</v>
+      </c>
+      <c r="F12" s="20">
+        <v>0</v>
+      </c>
+      <c r="G12" s="20">
+        <v>30</v>
       </c>
       <c r="H12" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I12" s="7">
         <v>0</v>
@@ -1004,28 +2281,28 @@
     </row>
     <row r="13" spans="1:20" ht="17.25" thickBot="1">
       <c r="A13" s="6">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="4">
         <v>2</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="7">
-        <v>0</v>
-      </c>
-      <c r="E13" s="7">
-        <v>0</v>
-      </c>
-      <c r="F13" s="7">
-        <v>0</v>
-      </c>
-      <c r="G13" s="7">
-        <v>10</v>
+      <c r="C13" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="20">
+        <v>0</v>
+      </c>
+      <c r="E13" s="20">
+        <v>0</v>
+      </c>
+      <c r="F13" s="20">
+        <v>1</v>
+      </c>
+      <c r="G13" s="20">
+        <v>20</v>
       </c>
       <c r="H13" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I13" s="7">
         <v>0</v>
@@ -1046,28 +2323,28 @@
     </row>
     <row r="14" spans="1:20" ht="17.25" thickBot="1">
       <c r="A14" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="4">
         <v>2</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="7">
-        <v>0</v>
-      </c>
-      <c r="E14" s="7">
-        <v>0</v>
-      </c>
-      <c r="F14" s="7">
-        <v>0</v>
-      </c>
-      <c r="G14" s="7">
-        <v>10</v>
+      <c r="C14" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="20">
+        <v>0</v>
+      </c>
+      <c r="E14" s="20">
+        <v>0</v>
+      </c>
+      <c r="F14" s="20">
+        <v>2</v>
+      </c>
+      <c r="G14" s="20">
+        <v>30</v>
       </c>
       <c r="H14" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I14" s="7">
         <v>0</v>
@@ -1088,28 +2365,28 @@
     </row>
     <row r="15" spans="1:20" ht="17.25" thickBot="1">
       <c r="A15" s="6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="4">
         <v>2</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="7">
-        <v>0</v>
-      </c>
-      <c r="E15" s="7">
-        <v>0</v>
-      </c>
-      <c r="F15" s="7">
-        <v>0</v>
-      </c>
-      <c r="G15" s="7">
-        <v>10</v>
+      <c r="C15" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="20">
+        <v>0</v>
+      </c>
+      <c r="E15" s="20">
+        <v>0</v>
+      </c>
+      <c r="F15" s="20">
+        <v>3</v>
+      </c>
+      <c r="G15" s="20">
+        <v>35</v>
       </c>
       <c r="H15" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I15" s="7">
         <v>0</v>
@@ -1130,28 +2407,28 @@
     </row>
     <row r="16" spans="1:20" ht="17.25" thickBot="1">
       <c r="A16" s="6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="4">
         <v>2</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="7">
-        <v>0</v>
-      </c>
-      <c r="E16" s="7">
-        <v>0</v>
-      </c>
-      <c r="F16" s="7">
-        <v>0</v>
-      </c>
-      <c r="G16" s="7">
-        <v>10</v>
+      <c r="C16" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="20">
+        <v>0</v>
+      </c>
+      <c r="E16" s="20">
+        <v>0</v>
+      </c>
+      <c r="F16" s="20">
+        <v>4</v>
+      </c>
+      <c r="G16" s="20">
+        <v>40</v>
       </c>
       <c r="H16" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I16" s="7">
         <v>0</v>
@@ -1172,28 +2449,28 @@
     </row>
     <row r="17" spans="1:20" ht="17.25" thickBot="1">
       <c r="A17" s="6">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="4">
         <v>2</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="7">
-        <v>0</v>
-      </c>
-      <c r="E17" s="7">
-        <v>0</v>
-      </c>
-      <c r="F17" s="7">
-        <v>0</v>
-      </c>
-      <c r="G17" s="7">
-        <v>10</v>
+      <c r="C17" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="20">
+        <v>0</v>
+      </c>
+      <c r="E17" s="20">
+        <v>0</v>
+      </c>
+      <c r="F17" s="20">
+        <v>5</v>
+      </c>
+      <c r="G17" s="20">
+        <v>50</v>
       </c>
       <c r="H17" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I17" s="7">
         <v>0</v>
@@ -1214,28 +2491,28 @@
     </row>
     <row r="18" spans="1:20" ht="17.25" thickBot="1">
       <c r="A18" s="6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="4">
         <v>2</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="7">
-        <v>0</v>
-      </c>
-      <c r="E18" s="7">
-        <v>0</v>
-      </c>
-      <c r="F18" s="7">
-        <v>0</v>
-      </c>
-      <c r="G18" s="7">
-        <v>10</v>
+      <c r="C18" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="20">
+        <v>0</v>
+      </c>
+      <c r="E18" s="20">
+        <v>0</v>
+      </c>
+      <c r="F18" s="20">
+        <v>6</v>
+      </c>
+      <c r="G18" s="20">
+        <v>40</v>
       </c>
       <c r="H18" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I18" s="7">
         <v>0</v>
@@ -1256,28 +2533,28 @@
     </row>
     <row r="19" spans="1:20" ht="17.25" thickBot="1">
       <c r="A19" s="6">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="4">
         <v>2</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="7">
-        <v>0</v>
-      </c>
-      <c r="E19" s="7">
-        <v>0</v>
-      </c>
-      <c r="F19" s="7">
-        <v>0</v>
-      </c>
-      <c r="G19" s="7">
-        <v>10</v>
+      <c r="C19" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="20">
+        <v>0</v>
+      </c>
+      <c r="E19" s="20">
+        <v>0</v>
+      </c>
+      <c r="F19" s="20">
+        <v>7</v>
+      </c>
+      <c r="G19" s="20">
+        <v>60</v>
       </c>
       <c r="H19" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I19" s="7">
         <v>0</v>
@@ -1298,34 +2575,34 @@
     </row>
     <row r="20" spans="1:20" ht="17.25" thickBot="1">
       <c r="A20" s="6">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="4">
         <v>2</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="20">
+        <v>0</v>
+      </c>
+      <c r="E20" s="20">
+        <v>0</v>
+      </c>
+      <c r="F20" s="20">
         <v>10</v>
       </c>
-      <c r="D20" s="7">
-        <v>0</v>
-      </c>
-      <c r="E20" s="7">
-        <v>0</v>
-      </c>
-      <c r="F20" s="7">
-        <v>0</v>
-      </c>
-      <c r="G20" s="7">
-        <v>10</v>
+      <c r="G20" s="20">
+        <v>50</v>
       </c>
       <c r="H20" s="7">
-        <v>5.5</v>
+        <v>50</v>
       </c>
       <c r="I20" s="7">
         <v>0</v>
       </c>
       <c r="J20" s="3">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
@@ -1340,34 +2617,34 @@
     </row>
     <row r="21" spans="1:20" ht="17.25" thickBot="1">
       <c r="A21" s="6">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" s="4">
         <v>2</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="20">
+        <v>0</v>
+      </c>
+      <c r="E21" s="20">
+        <v>0</v>
+      </c>
+      <c r="F21" s="20">
         <v>11</v>
       </c>
-      <c r="D21" s="7">
-        <v>0</v>
-      </c>
-      <c r="E21" s="7">
-        <v>0</v>
-      </c>
-      <c r="F21" s="7">
-        <v>0</v>
-      </c>
-      <c r="G21" s="7">
-        <v>10</v>
+      <c r="G21" s="20">
+        <v>15</v>
       </c>
       <c r="H21" s="7">
-        <v>5.5</v>
+        <v>20</v>
       </c>
       <c r="I21" s="7">
         <v>0</v>
       </c>
       <c r="J21" s="3">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
@@ -1382,28 +2659,28 @@
     </row>
     <row r="22" spans="1:20" ht="17.25" thickBot="1">
       <c r="A22" s="6">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" s="4">
         <v>3</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="7">
-        <v>0</v>
-      </c>
-      <c r="E22" s="7">
-        <v>0</v>
-      </c>
-      <c r="F22" s="7">
-        <v>0</v>
-      </c>
-      <c r="G22" s="7">
-        <v>10</v>
+      <c r="C22" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="18">
+        <v>0</v>
+      </c>
+      <c r="E22" s="18">
+        <v>0</v>
+      </c>
+      <c r="F22" s="18">
+        <v>0</v>
+      </c>
+      <c r="G22" s="18">
+        <v>50</v>
       </c>
       <c r="H22" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I22" s="7">
         <v>0</v>
@@ -1424,28 +2701,28 @@
     </row>
     <row r="23" spans="1:20" ht="17.25" thickBot="1">
       <c r="A23" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" s="4">
         <v>3</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="7">
-        <v>0</v>
-      </c>
-      <c r="E23" s="7">
-        <v>0</v>
-      </c>
-      <c r="F23" s="7">
-        <v>0</v>
-      </c>
-      <c r="G23" s="7">
-        <v>10</v>
+      <c r="C23" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="18">
+        <v>0</v>
+      </c>
+      <c r="E23" s="18">
+        <v>0</v>
+      </c>
+      <c r="F23" s="18">
+        <v>1</v>
+      </c>
+      <c r="G23" s="18">
+        <v>60</v>
       </c>
       <c r="H23" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I23" s="7">
         <v>0</v>
@@ -1466,28 +2743,28 @@
     </row>
     <row r="24" spans="1:20" ht="17.25" thickBot="1">
       <c r="A24" s="6">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" s="4">
         <v>3</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="7">
-        <v>0</v>
-      </c>
-      <c r="E24" s="7">
-        <v>0</v>
-      </c>
-      <c r="F24" s="7">
-        <v>0</v>
-      </c>
-      <c r="G24" s="7">
-        <v>10</v>
+      <c r="C24" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="18">
+        <v>0</v>
+      </c>
+      <c r="E24" s="18">
+        <v>0</v>
+      </c>
+      <c r="F24" s="18">
+        <v>2</v>
+      </c>
+      <c r="G24" s="18">
+        <v>50</v>
       </c>
       <c r="H24" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I24" s="7">
         <v>0</v>
@@ -1508,28 +2785,28 @@
     </row>
     <row r="25" spans="1:20" ht="17.25" thickBot="1">
       <c r="A25" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" s="4">
         <v>3</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="7">
-        <v>0</v>
-      </c>
-      <c r="E25" s="7">
-        <v>0</v>
-      </c>
-      <c r="F25" s="7">
-        <v>0</v>
-      </c>
-      <c r="G25" s="7">
-        <v>10</v>
+      <c r="C25" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="18">
+        <v>0</v>
+      </c>
+      <c r="E25" s="18">
+        <v>0</v>
+      </c>
+      <c r="F25" s="18">
+        <v>12</v>
+      </c>
+      <c r="G25" s="18">
+        <v>15</v>
       </c>
       <c r="H25" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I25" s="7">
         <v>0</v>
@@ -1550,28 +2827,28 @@
     </row>
     <row r="26" spans="1:20" ht="17.25" thickBot="1">
       <c r="A26" s="6">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" s="4">
         <v>3</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="7">
-        <v>0</v>
-      </c>
-      <c r="E26" s="7">
-        <v>0</v>
-      </c>
-      <c r="F26" s="7">
-        <v>0</v>
-      </c>
-      <c r="G26" s="7">
-        <v>10</v>
+      <c r="C26" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="18">
+        <v>0</v>
+      </c>
+      <c r="E26" s="18">
+        <v>0</v>
+      </c>
+      <c r="F26" s="18">
+        <v>4</v>
+      </c>
+      <c r="G26" s="18">
+        <v>70</v>
       </c>
       <c r="H26" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I26" s="7">
         <v>0</v>
@@ -1592,28 +2869,28 @@
     </row>
     <row r="27" spans="1:20" ht="17.25" thickBot="1">
       <c r="A27" s="6">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" s="4">
         <v>3</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="7">
-        <v>0</v>
-      </c>
-      <c r="E27" s="7">
-        <v>0</v>
-      </c>
-      <c r="F27" s="7">
-        <v>0</v>
-      </c>
-      <c r="G27" s="7">
-        <v>10</v>
+      <c r="C27" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="18">
+        <v>0</v>
+      </c>
+      <c r="E27" s="18">
+        <v>0</v>
+      </c>
+      <c r="F27" s="18">
+        <v>13</v>
+      </c>
+      <c r="G27" s="18">
+        <v>100</v>
       </c>
       <c r="H27" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I27" s="7">
         <v>0</v>
@@ -1634,28 +2911,28 @@
     </row>
     <row r="28" spans="1:20" ht="17.25" thickBot="1">
       <c r="A28" s="6">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" s="4">
         <v>3</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="7">
-        <v>0</v>
-      </c>
-      <c r="E28" s="7">
-        <v>0</v>
-      </c>
-      <c r="F28" s="7">
-        <v>0</v>
-      </c>
-      <c r="G28" s="7">
-        <v>10</v>
+      <c r="C28" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="18">
+        <v>0</v>
+      </c>
+      <c r="E28" s="18">
+        <v>0</v>
+      </c>
+      <c r="F28" s="18">
+        <v>14</v>
+      </c>
+      <c r="G28" s="18">
+        <v>100</v>
       </c>
       <c r="H28" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I28" s="7">
         <v>0</v>
@@ -1676,28 +2953,28 @@
     </row>
     <row r="29" spans="1:20" ht="17.25" thickBot="1">
       <c r="A29" s="6">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" s="4">
         <v>3</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="7">
-        <v>0</v>
-      </c>
-      <c r="E29" s="7">
-        <v>0</v>
-      </c>
-      <c r="F29" s="7">
-        <v>0</v>
-      </c>
-      <c r="G29" s="7">
-        <v>10</v>
+      <c r="C29" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="18">
+        <v>0</v>
+      </c>
+      <c r="E29" s="18">
+        <v>0</v>
+      </c>
+      <c r="F29" s="18">
+        <v>15</v>
+      </c>
+      <c r="G29" s="18">
+        <v>100</v>
       </c>
       <c r="H29" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I29" s="7">
         <v>0</v>
@@ -1718,34 +2995,34 @@
     </row>
     <row r="30" spans="1:20" ht="17.25" thickBot="1">
       <c r="A30" s="6">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" s="4">
         <v>3</v>
       </c>
-      <c r="C30" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="7">
-        <v>0</v>
-      </c>
-      <c r="E30" s="7">
-        <v>0</v>
-      </c>
-      <c r="F30" s="7">
-        <v>0</v>
-      </c>
-      <c r="G30" s="7">
-        <v>10</v>
+      <c r="C30" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="18">
+        <v>0</v>
+      </c>
+      <c r="E30" s="18">
+        <v>0</v>
+      </c>
+      <c r="F30" s="18">
+        <v>16</v>
+      </c>
+      <c r="G30" s="18">
+        <v>200</v>
       </c>
       <c r="H30" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I30" s="7">
         <v>0</v>
       </c>
       <c r="J30" s="3">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
@@ -1760,34 +3037,34 @@
     </row>
     <row r="31" spans="1:20" ht="17.25" thickBot="1">
       <c r="A31" s="6">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" s="4">
         <v>3</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="7">
-        <v>0</v>
-      </c>
-      <c r="E31" s="7">
-        <v>0</v>
-      </c>
-      <c r="F31" s="7">
-        <v>0</v>
-      </c>
-      <c r="G31" s="7">
-        <v>10</v>
+      <c r="C31" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="18">
+        <v>0</v>
+      </c>
+      <c r="E31" s="18">
+        <v>0</v>
+      </c>
+      <c r="F31" s="18">
+        <v>17</v>
+      </c>
+      <c r="G31" s="18">
+        <v>5</v>
       </c>
       <c r="H31" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I31" s="7">
         <v>0</v>
       </c>
       <c r="J31" s="3">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
@@ -1802,28 +3079,28 @@
     </row>
     <row r="32" spans="1:20" ht="17.25" thickBot="1">
       <c r="A32" s="6">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" s="4">
         <v>4</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="16">
+        <v>0</v>
+      </c>
+      <c r="E32" s="16">
+        <v>0</v>
+      </c>
+      <c r="F32" s="16">
+        <v>18</v>
+      </c>
+      <c r="G32" s="16">
+        <v>50</v>
+      </c>
+      <c r="H32" s="7">
         <v>10</v>
-      </c>
-      <c r="D32" s="7">
-        <v>0</v>
-      </c>
-      <c r="E32" s="7">
-        <v>0</v>
-      </c>
-      <c r="F32" s="7">
-        <v>0</v>
-      </c>
-      <c r="G32" s="7">
-        <v>10</v>
-      </c>
-      <c r="H32" s="7">
-        <v>5.5</v>
       </c>
       <c r="I32" s="7">
         <v>0</v>
@@ -1844,28 +3121,28 @@
     </row>
     <row r="33" spans="1:20" ht="17.25" thickBot="1">
       <c r="A33" s="6">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="4">
         <v>4</v>
       </c>
-      <c r="C33" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="7">
-        <v>0</v>
-      </c>
-      <c r="E33" s="7">
-        <v>0</v>
-      </c>
-      <c r="F33" s="7">
-        <v>0</v>
-      </c>
-      <c r="G33" s="7">
-        <v>10</v>
+      <c r="C33" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="16">
+        <v>0</v>
+      </c>
+      <c r="E33" s="16">
+        <v>0</v>
+      </c>
+      <c r="F33" s="16">
+        <v>19</v>
+      </c>
+      <c r="G33" s="16">
+        <v>60</v>
       </c>
       <c r="H33" s="7">
-        <v>5.5</v>
+        <v>20</v>
       </c>
       <c r="I33" s="7">
         <v>0</v>
@@ -1886,28 +3163,28 @@
     </row>
     <row r="34" spans="1:20" ht="17.25" thickBot="1">
       <c r="A34" s="6">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" s="4">
         <v>4</v>
       </c>
-      <c r="C34" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" s="7">
-        <v>0</v>
-      </c>
-      <c r="E34" s="7">
-        <v>0</v>
-      </c>
-      <c r="F34" s="7">
-        <v>0</v>
-      </c>
-      <c r="G34" s="7">
-        <v>10</v>
+      <c r="C34" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="16">
+        <v>0</v>
+      </c>
+      <c r="E34" s="16">
+        <v>0</v>
+      </c>
+      <c r="F34" s="16">
+        <v>20</v>
+      </c>
+      <c r="G34" s="16">
+        <v>50</v>
       </c>
       <c r="H34" s="7">
-        <v>5.5</v>
+        <v>100</v>
       </c>
       <c r="I34" s="7">
         <v>0</v>
@@ -1928,28 +3205,28 @@
     </row>
     <row r="35" spans="1:20" ht="17.25" thickBot="1">
       <c r="A35" s="6">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" s="4">
         <v>4</v>
       </c>
-      <c r="C35" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" s="7">
-        <v>0</v>
-      </c>
-      <c r="E35" s="7">
-        <v>0</v>
-      </c>
-      <c r="F35" s="7">
-        <v>0</v>
-      </c>
-      <c r="G35" s="7">
-        <v>10</v>
+      <c r="C35" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" s="16">
+        <v>0</v>
+      </c>
+      <c r="E35" s="16">
+        <v>0</v>
+      </c>
+      <c r="F35" s="16">
+        <v>21</v>
+      </c>
+      <c r="G35" s="16">
+        <v>100</v>
       </c>
       <c r="H35" s="7">
-        <v>5.5</v>
+        <v>50</v>
       </c>
       <c r="I35" s="7">
         <v>0</v>
@@ -1970,28 +3247,28 @@
     </row>
     <row r="36" spans="1:20" ht="17.25" thickBot="1">
       <c r="A36" s="6">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" s="4">
         <v>4</v>
       </c>
-      <c r="C36" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="7">
-        <v>0</v>
-      </c>
-      <c r="E36" s="7">
-        <v>0</v>
-      </c>
-      <c r="F36" s="7">
-        <v>0</v>
-      </c>
-      <c r="G36" s="7">
-        <v>10</v>
+      <c r="C36" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" s="16">
+        <v>0</v>
+      </c>
+      <c r="E36" s="16">
+        <v>0</v>
+      </c>
+      <c r="F36" s="16">
+        <v>22</v>
+      </c>
+      <c r="G36" s="16">
+        <v>100</v>
       </c>
       <c r="H36" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I36" s="7">
         <v>0</v>
@@ -2012,28 +3289,28 @@
     </row>
     <row r="37" spans="1:20" ht="17.25" thickBot="1">
       <c r="A37" s="6">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B37" s="4">
         <v>4</v>
       </c>
-      <c r="C37" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="7">
-        <v>0</v>
-      </c>
-      <c r="E37" s="7">
-        <v>0</v>
-      </c>
-      <c r="F37" s="7">
-        <v>0</v>
-      </c>
-      <c r="G37" s="7">
-        <v>10</v>
+      <c r="C37" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D37" s="16">
+        <v>0</v>
+      </c>
+      <c r="E37" s="16">
+        <v>0</v>
+      </c>
+      <c r="F37" s="16">
+        <v>23</v>
+      </c>
+      <c r="G37" s="16">
+        <v>100</v>
       </c>
       <c r="H37" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I37" s="7">
         <v>0</v>
@@ -2054,28 +3331,28 @@
     </row>
     <row r="38" spans="1:20" ht="17.25" thickBot="1">
       <c r="A38" s="6">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" s="4">
         <v>4</v>
       </c>
-      <c r="C38" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D38" s="7">
-        <v>0</v>
-      </c>
-      <c r="E38" s="7">
-        <v>0</v>
-      </c>
-      <c r="F38" s="7">
-        <v>0</v>
-      </c>
-      <c r="G38" s="7">
-        <v>10</v>
+      <c r="C38" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" s="16">
+        <v>0</v>
+      </c>
+      <c r="E38" s="16">
+        <v>0</v>
+      </c>
+      <c r="F38" s="16">
+        <v>24</v>
+      </c>
+      <c r="G38" s="16">
+        <v>30</v>
       </c>
       <c r="H38" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I38" s="7">
         <v>0</v>
@@ -2096,28 +3373,28 @@
     </row>
     <row r="39" spans="1:20" ht="17.25" thickBot="1">
       <c r="A39" s="6">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B39" s="4">
         <v>4</v>
       </c>
-      <c r="C39" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="7">
-        <v>0</v>
-      </c>
-      <c r="E39" s="7">
-        <v>0</v>
-      </c>
-      <c r="F39" s="7">
-        <v>0</v>
-      </c>
-      <c r="G39" s="7">
-        <v>10</v>
+      <c r="C39" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D39" s="16">
+        <v>0</v>
+      </c>
+      <c r="E39" s="16">
+        <v>0</v>
+      </c>
+      <c r="F39" s="16">
+        <v>25</v>
+      </c>
+      <c r="G39" s="16">
+        <v>100</v>
       </c>
       <c r="H39" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I39" s="7">
         <v>0</v>
@@ -2138,34 +3415,34 @@
     </row>
     <row r="40" spans="1:20" ht="17.25" thickBot="1">
       <c r="A40" s="6">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B40" s="4">
         <v>4</v>
       </c>
-      <c r="C40" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" s="7">
-        <v>0</v>
-      </c>
-      <c r="E40" s="7">
-        <v>0</v>
-      </c>
-      <c r="F40" s="7">
-        <v>0</v>
-      </c>
-      <c r="G40" s="7">
-        <v>10</v>
+      <c r="C40" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="16">
+        <v>0</v>
+      </c>
+      <c r="E40" s="16">
+        <v>0</v>
+      </c>
+      <c r="F40" s="16">
+        <v>4</v>
+      </c>
+      <c r="G40" s="16">
+        <v>100</v>
       </c>
       <c r="H40" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I40" s="7">
         <v>0</v>
       </c>
       <c r="J40" s="3">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
@@ -2180,34 +3457,34 @@
     </row>
     <row r="41" spans="1:20" ht="17.25" thickBot="1">
       <c r="A41" s="6">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B41" s="4">
         <v>4</v>
       </c>
-      <c r="C41" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" s="7">
-        <v>0</v>
-      </c>
-      <c r="E41" s="7">
-        <v>0</v>
-      </c>
-      <c r="F41" s="7">
-        <v>0</v>
-      </c>
-      <c r="G41" s="7">
-        <v>10</v>
+      <c r="C41" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" s="16">
+        <v>0</v>
+      </c>
+      <c r="E41" s="16">
+        <v>0</v>
+      </c>
+      <c r="F41" s="16">
+        <v>26</v>
+      </c>
+      <c r="G41" s="16">
+        <v>100</v>
       </c>
       <c r="H41" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="I41" s="7">
         <v>0</v>
       </c>
       <c r="J41" s="3">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
@@ -2222,34 +3499,642 @@
     </row>
     <row r="42" spans="1:20" ht="17.25" thickBot="1">
       <c r="A42" s="6">
+        <v>41</v>
+      </c>
+      <c r="B42" s="4">
+        <v>5</v>
+      </c>
+      <c r="C42" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" s="22">
+        <v>0</v>
+      </c>
+      <c r="E42" s="22">
+        <v>0</v>
+      </c>
+      <c r="F42" s="22">
+        <v>27</v>
+      </c>
+      <c r="G42" s="22">
+        <v>20</v>
+      </c>
+      <c r="H42" s="7">
+        <v>0</v>
+      </c>
+      <c r="I42" s="7">
+        <v>0</v>
+      </c>
+      <c r="J42" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" ht="17.25" thickBot="1">
+      <c r="A43" s="6">
+        <v>42</v>
+      </c>
+      <c r="B43" s="25">
+        <v>5</v>
+      </c>
+      <c r="C43" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" s="26">
+        <v>0</v>
+      </c>
+      <c r="E43" s="22">
+        <v>0</v>
+      </c>
+      <c r="F43" s="22">
+        <v>28</v>
+      </c>
+      <c r="G43" s="22">
+        <v>300</v>
+      </c>
+      <c r="H43" s="7">
+        <v>300</v>
+      </c>
+      <c r="I43" s="7">
+        <v>0</v>
+      </c>
+      <c r="J43" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" ht="17.25" thickBot="1">
+      <c r="A44" s="6">
+        <v>43</v>
+      </c>
+      <c r="B44" s="25">
+        <v>5</v>
+      </c>
+      <c r="C44" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" s="26">
+        <v>0</v>
+      </c>
+      <c r="E44" s="22">
+        <v>0</v>
+      </c>
+      <c r="F44" s="22">
+        <v>29</v>
+      </c>
+      <c r="G44" s="22">
+        <v>30</v>
+      </c>
+      <c r="H44" s="7">
+        <v>0</v>
+      </c>
+      <c r="I44" s="7">
+        <v>0</v>
+      </c>
+      <c r="J44" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" ht="17.25" thickBot="1">
+      <c r="A45" s="6">
+        <v>44</v>
+      </c>
+      <c r="B45" s="25">
+        <v>5</v>
+      </c>
+      <c r="C45" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D45" s="26">
+        <v>0</v>
+      </c>
+      <c r="E45" s="22">
+        <v>0</v>
+      </c>
+      <c r="F45" s="22">
+        <v>30</v>
+      </c>
+      <c r="G45" s="22">
+        <v>200</v>
+      </c>
+      <c r="H45" s="7">
+        <v>30</v>
+      </c>
+      <c r="I45" s="7">
+        <v>0</v>
+      </c>
+      <c r="J45" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" ht="17.25" thickBot="1">
+      <c r="A46" s="6">
+        <v>45</v>
+      </c>
+      <c r="B46" s="25">
+        <v>5</v>
+      </c>
+      <c r="C46" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D46" s="26">
+        <v>0</v>
+      </c>
+      <c r="E46" s="22">
+        <v>0</v>
+      </c>
+      <c r="F46" s="22">
+        <v>31</v>
+      </c>
+      <c r="G46" s="22">
+        <v>300</v>
+      </c>
+      <c r="H46" s="7">
+        <v>0</v>
+      </c>
+      <c r="I46" s="7">
+        <v>0</v>
+      </c>
+      <c r="J46" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" ht="17.25" thickBot="1">
+      <c r="A47" s="6">
+        <v>46</v>
+      </c>
+      <c r="B47" s="25">
+        <v>5</v>
+      </c>
+      <c r="C47" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" s="26">
+        <v>0</v>
+      </c>
+      <c r="E47" s="22">
+        <v>0</v>
+      </c>
+      <c r="F47" s="22">
+        <v>32</v>
+      </c>
+      <c r="G47" s="22">
+        <v>1</v>
+      </c>
+      <c r="H47" s="7">
+        <v>0</v>
+      </c>
+      <c r="I47" s="7">
+        <v>0</v>
+      </c>
+      <c r="J47" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" ht="17.25" thickBot="1">
+      <c r="A48" s="6">
+        <v>47</v>
+      </c>
+      <c r="B48" s="25">
+        <v>5</v>
+      </c>
+      <c r="C48" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="D48" s="26">
+        <v>0</v>
+      </c>
+      <c r="E48" s="22">
+        <v>0</v>
+      </c>
+      <c r="F48" s="22">
+        <v>33</v>
+      </c>
+      <c r="G48" s="22">
+        <v>50</v>
+      </c>
+      <c r="H48" s="7">
+        <v>0</v>
+      </c>
+      <c r="I48" s="7">
+        <v>0</v>
+      </c>
+      <c r="J48" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="17.25" thickBot="1">
+      <c r="A49" s="6">
+        <v>48</v>
+      </c>
+      <c r="B49" s="25">
+        <v>5</v>
+      </c>
+      <c r="C49" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D49" s="26">
+        <v>0</v>
+      </c>
+      <c r="E49" s="22">
+        <v>0</v>
+      </c>
+      <c r="F49" s="22">
+        <v>2</v>
+      </c>
+      <c r="G49" s="22">
+        <v>100</v>
+      </c>
+      <c r="H49" s="7">
+        <v>0</v>
+      </c>
+      <c r="I49" s="7">
+        <v>0</v>
+      </c>
+      <c r="J49" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="17.25" thickBot="1">
+      <c r="A50" s="6">
+        <v>49</v>
+      </c>
+      <c r="B50" s="25">
+        <v>5</v>
+      </c>
+      <c r="C50" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D50" s="26">
+        <v>0</v>
+      </c>
+      <c r="E50" s="22">
+        <v>0</v>
+      </c>
+      <c r="F50" s="22">
+        <v>34</v>
+      </c>
+      <c r="G50" s="22">
+        <v>100</v>
+      </c>
+      <c r="H50" s="7">
+        <v>0</v>
+      </c>
+      <c r="I50" s="7">
+        <v>0</v>
+      </c>
+      <c r="J50" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="17.25" thickBot="1">
+      <c r="A51" s="6">
+        <v>50</v>
+      </c>
+      <c r="B51" s="25">
+        <v>5</v>
+      </c>
+      <c r="C51" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D51" s="26">
+        <v>0</v>
+      </c>
+      <c r="E51" s="22">
+        <v>0</v>
+      </c>
+      <c r="F51" s="22">
+        <v>35</v>
+      </c>
+      <c r="G51" s="22">
+        <v>100</v>
+      </c>
+      <c r="H51" s="7">
+        <v>0</v>
+      </c>
+      <c r="I51" s="7">
+        <v>0</v>
+      </c>
+      <c r="J51" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="17.25" thickBot="1">
+      <c r="A52" s="6">
+        <v>51</v>
+      </c>
+      <c r="B52" s="23">
+        <v>6</v>
+      </c>
+      <c r="C52" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D52" s="24">
+        <v>0</v>
+      </c>
+      <c r="E52" s="24">
+        <v>0</v>
+      </c>
+      <c r="F52" s="24">
+        <v>36</v>
+      </c>
+      <c r="G52" s="24">
+        <v>100</v>
+      </c>
+      <c r="H52" s="7">
+        <v>100</v>
+      </c>
+      <c r="I52" s="7">
+        <v>0</v>
+      </c>
+      <c r="J52" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="17.25" thickBot="1">
+      <c r="A53" s="6">
+        <v>52</v>
+      </c>
+      <c r="B53" s="23">
+        <v>6</v>
+      </c>
+      <c r="C53" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="D53" s="24">
+        <v>0</v>
+      </c>
+      <c r="E53" s="24">
+        <v>0</v>
+      </c>
+      <c r="F53" s="24">
+        <v>37</v>
+      </c>
+      <c r="G53" s="24">
+        <v>0</v>
+      </c>
+      <c r="H53" s="7">
+        <v>0</v>
+      </c>
+      <c r="I53" s="7">
+        <v>0</v>
+      </c>
+      <c r="J53" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="17.25" thickBot="1">
+      <c r="A54" s="6">
+        <v>53</v>
+      </c>
+      <c r="B54" s="23">
+        <v>6</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D54" s="24">
+        <v>0</v>
+      </c>
+      <c r="E54" s="24">
+        <v>0</v>
+      </c>
+      <c r="F54" s="24">
+        <v>17</v>
+      </c>
+      <c r="G54" s="24">
+        <v>3</v>
+      </c>
+      <c r="H54" s="7">
+        <v>0</v>
+      </c>
+      <c r="I54" s="7">
+        <v>0</v>
+      </c>
+      <c r="J54" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="17.25" thickBot="1">
+      <c r="A55" s="6">
+        <v>54</v>
+      </c>
+      <c r="B55" s="23">
+        <v>6</v>
+      </c>
+      <c r="C55" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="D55" s="24">
+        <v>0</v>
+      </c>
+      <c r="E55" s="24">
+        <v>0</v>
+      </c>
+      <c r="F55" s="24">
+        <v>38</v>
+      </c>
+      <c r="G55" s="24">
+        <v>30</v>
+      </c>
+      <c r="H55" s="7">
+        <v>0</v>
+      </c>
+      <c r="I55" s="7">
+        <v>0</v>
+      </c>
+      <c r="J55" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="17.25" thickBot="1">
+      <c r="A56" s="6">
+        <v>55</v>
+      </c>
+      <c r="B56" s="23">
+        <v>6</v>
+      </c>
+      <c r="C56" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="D56" s="24">
+        <v>0</v>
+      </c>
+      <c r="E56" s="24">
+        <v>0</v>
+      </c>
+      <c r="F56" s="24">
+        <v>39</v>
+      </c>
+      <c r="G56" s="24">
+        <v>30</v>
+      </c>
+      <c r="H56" s="7">
+        <v>0</v>
+      </c>
+      <c r="I56" s="7">
+        <v>0</v>
+      </c>
+      <c r="J56" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="17.25" thickBot="1">
+      <c r="A57" s="6">
+        <v>56</v>
+      </c>
+      <c r="B57" s="23">
+        <v>6</v>
+      </c>
+      <c r="C57" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D57" s="24">
+        <v>0</v>
+      </c>
+      <c r="E57" s="24">
+        <v>0</v>
+      </c>
+      <c r="F57" s="24">
         <v>40</v>
       </c>
-      <c r="B42" s="4">
+      <c r="G57" s="24">
+        <v>100</v>
+      </c>
+      <c r="H57" s="7">
+        <v>99</v>
+      </c>
+      <c r="I57" s="7">
+        <v>100</v>
+      </c>
+      <c r="J57" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="17.25" thickBot="1">
+      <c r="A58" s="6">
+        <v>57</v>
+      </c>
+      <c r="B58" s="23">
         <v>6</v>
       </c>
-      <c r="C42" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" s="7">
-        <v>0</v>
-      </c>
-      <c r="E42" s="7">
-        <v>0</v>
-      </c>
-      <c r="F42" s="7">
-        <v>0</v>
-      </c>
-      <c r="G42" s="7">
+      <c r="C58" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D58" s="24">
+        <v>0</v>
+      </c>
+      <c r="E58" s="24">
+        <v>0</v>
+      </c>
+      <c r="F58" s="24">
+        <v>41</v>
+      </c>
+      <c r="G58" s="24">
         <v>10</v>
       </c>
-      <c r="H42" s="7">
-        <v>5.5</v>
-      </c>
-      <c r="I42" s="7">
-        <v>0</v>
-      </c>
-      <c r="J42" s="3">
-        <v>12</v>
+      <c r="H58" s="7">
+        <v>0</v>
+      </c>
+      <c r="I58" s="7">
+        <v>0</v>
+      </c>
+      <c r="J58" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="17.25" thickBot="1">
+      <c r="A59" s="6">
+        <v>58</v>
+      </c>
+      <c r="B59" s="23">
+        <v>6</v>
+      </c>
+      <c r="C59" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D59" s="24">
+        <v>0</v>
+      </c>
+      <c r="E59" s="24">
+        <v>0</v>
+      </c>
+      <c r="F59" s="24">
+        <v>42</v>
+      </c>
+      <c r="G59" s="24">
+        <v>0</v>
+      </c>
+      <c r="H59" s="7">
+        <v>0</v>
+      </c>
+      <c r="I59" s="7">
+        <v>0</v>
+      </c>
+      <c r="J59" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="17.25" thickBot="1">
+      <c r="A60" s="6">
+        <v>59</v>
+      </c>
+      <c r="B60" s="23">
+        <v>6</v>
+      </c>
+      <c r="C60" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D60" s="24">
+        <v>0</v>
+      </c>
+      <c r="E60" s="24">
+        <v>0</v>
+      </c>
+      <c r="F60" s="24">
+        <v>29</v>
+      </c>
+      <c r="G60" s="24">
+        <v>100</v>
+      </c>
+      <c r="H60" s="7">
+        <v>0</v>
+      </c>
+      <c r="I60" s="7">
+        <v>0</v>
+      </c>
+      <c r="J60" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="17.25" thickBot="1">
+      <c r="A61" s="6">
+        <v>60</v>
+      </c>
+      <c r="B61" s="23">
+        <v>6</v>
+      </c>
+      <c r="C61" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D61" s="24">
+        <v>0</v>
+      </c>
+      <c r="E61" s="24">
+        <v>0</v>
+      </c>
+      <c r="F61" s="24">
+        <v>12</v>
+      </c>
+      <c r="G61" s="24">
+        <v>90</v>
+      </c>
+      <c r="H61" s="7">
+        <v>0</v>
+      </c>
+      <c r="I61" s="7">
+        <v>0</v>
+      </c>
+      <c r="J61" s="3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>